<commit_message>
Parametrización de Evaluación financiera y proyección de ventas
Parametrización de Evaluación financiera y proyección de ventas.
</commit_message>
<xml_diff>
--- a/project/Documents/02. AUTOMATION SOLUTIOS ( AUTOSOL) - EVALUACION FINANCIERA.xlsx
+++ b/project/Documents/02. AUTOMATION SOLUTIOS ( AUTOSOL) - EVALUACION FINANCIERA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yovan\Desktop\APM\ausol-apm.github.io\project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\ausol-apm.github.io\project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1FAFE2-DEC4-4852-9965-7EDCB30454CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C9D1E7-5ED8-4B60-9DB6-D617DDDE6EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyección ventas" sheetId="2" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Ventas Mensual</t>
   </si>
   <si>
-    <t>Producción máxima (Unidades)</t>
-  </si>
-  <si>
     <t>Distribución Mensual de ventas estimada:</t>
   </si>
   <si>
@@ -328,21 +325,30 @@
   <si>
     <t>INVERSION EN INGENIERÍA AUTOMATIZACIÓN</t>
   </si>
+  <si>
+    <t>Turnos por día</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producción máxima (Unidades) al día </t>
+  </si>
+  <si>
+    <t>Producción máxima (unidades) por turno</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="[$$-240A]\ #,##0.00"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="[$$-240A]\ #,##0.00"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -559,14 +565,14 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,36 +587,35 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -634,28 +639,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -673,6 +678,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -736,7 +750,11 @@
             </a:r>
             <a:r>
               <a:rPr lang="es-MX" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t> </a:t>
+              <a:t>  </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>en Colombia</a:t>
             </a:r>
             <a:endParaRPr lang="es-MX"/>
           </a:p>
@@ -1428,7 +1446,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-MX" b="1"/>
-              <a:t>Estimación ventas mensuales por tipo de juguete (Unidades)</a:t>
+              <a:t>Estimación ventas mensuales por tipo de juguete (Unidades) en Colombia</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2243,40 +2261,40 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5851.4285714285725</c:v>
+                  <c:v>14628.571428571429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5851.4285714285725</c:v>
+                  <c:v>14628.571428571429</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7478.4285714285761</c:v>
+                  <c:v>21668.571428571435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14757</c:v>
+                  <c:v>33920</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3644.095238095244</c:v>
+                  <c:v>14628.57142857142</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14757</c:v>
+                  <c:v>34133.333333333343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14757</c:v>
+                  <c:v>34133.333333333343</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10408.952380952396</c:v>
+                  <c:v>37912.380952380976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14757</c:v>
+                  <c:v>33920</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14757</c:v>
+                  <c:v>33920</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14757</c:v>
+                  <c:v>33920</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14757</c:v>
+                  <c:v>33920</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2365,40 +2383,40 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4266.666666666667</c:v>
+                  <c:v>10666.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4266.666666666667</c:v>
+                  <c:v>10666.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4266.666666666667</c:v>
+                  <c:v>10666.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11946.666666666668</c:v>
+                  <c:v>29866.666666666668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4266.666666666667</c:v>
+                  <c:v>10666.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9955.5555555555566</c:v>
+                  <c:v>24888.888888888891</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9955.5555555555566</c:v>
+                  <c:v>24888.888888888891</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4266.666666666667</c:v>
+                  <c:v>10666.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7745.4444444444453</c:v>
+                  <c:v>27171.111111111109</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12873</c:v>
+                  <c:v>29580</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12873</c:v>
+                  <c:v>29580</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12873</c:v>
+                  <c:v>29580</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2487,40 +2505,40 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2438.0952380952381</c:v>
+                  <c:v>6095.2380952380954</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2438.0952380952381</c:v>
+                  <c:v>6095.2380952380954</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2438.0952380952381</c:v>
+                  <c:v>6095.2380952380954</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6826.6666666666679</c:v>
+                  <c:v>17066.666666666668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2438.0952380952381</c:v>
+                  <c:v>6095.2380952380954</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5688.8888888888905</c:v>
+                  <c:v>14222.222222222224</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5688.8888888888905</c:v>
+                  <c:v>14222.222222222224</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2438.0952380952381</c:v>
+                  <c:v>6095.2380952380954</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2438.0952380952381</c:v>
+                  <c:v>6095.2380952380954</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5883.8730158730177</c:v>
+                  <c:v>18379.682539682544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9086</c:v>
+                  <c:v>20880</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9086</c:v>
+                  <c:v>20880</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2802,6 +2820,774 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Ventas mensuales proyectadas por tipo de juguete dada la producción máxima de la planta automatizada (Millones COP)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Proyección ventas'!$B$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Moto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Proyección ventas'!$A$51:$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Proyección ventas'!$B$51:$B$62</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>409.60000000000008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>341.33333333333343</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>341.33333333333343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>273.06666666666672</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>146.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024.0000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D42B-4E41-8BCF-A14F463F9EB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Proyección ventas'!$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Barco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Proyección ventas'!$A$51:$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Proyección ventas'!$C$51:$C$62</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>358.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>298.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>298.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238.93333333333334</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>895.99999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D42B-4E41-8BCF-A14F463F9EB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Proyección ventas'!$D$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Casa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Proyección ventas'!$A$51:$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Proyección ventas'!$D$51:$D$62</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>213.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>213.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>170.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>640</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D42B-4E41-8BCF-A14F463F9EB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1793516320"/>
+        <c:axId val="1793523520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1793516320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1793523520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1793523520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Millones de pesos COP</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1793516320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2891,7 +3677,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-1030000000</c:v>
+                  <c:v>-1016000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2922,7 +3708,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2953,7 +3739,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2984,7 +3770,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3015,7 +3801,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>200116799.97868001</c:v>
+                  <c:v>524342000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3046,7 +3832,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3079,7 +3865,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163730666.6489</c:v>
+                  <c:v>433376666.66666675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3112,7 +3898,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163730666.6489</c:v>
+                  <c:v>433376666.66666675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3145,7 +3931,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3178,7 +3964,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3211,7 +3997,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>127344533.31912</c:v>
+                  <c:v>342411333.33333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3244,7 +4030,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60030186.659026988</c:v>
+                  <c:v>174125466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3278,7 +4064,7 @@
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>527591999.94669992</c:v>
+                  <c:v>1343030000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3580,6 +4366,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5129,7 +5955,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5237,6 +6063,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5247,6 +6078,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5278,6 +6114,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5631,17 +6470,520 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>617220</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -5671,13 +7013,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -5707,13 +7049,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -5736,6 +7078,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>678180</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D80A82-F935-AA87-41E6-0E7133B51743}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6050,351 +7428,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C25875F-8E18-430B-8568-E6400B7C666D}">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" customWidth="1"/>
-    <col min="13" max="13" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+    <row r="1" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="46"/>
+      <c r="P2" s="45"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="26">
-        <f>G15*I3*N7%</f>
+      <c r="B3" s="25">
+        <f>G15*I3*P7%</f>
         <v>292.57142857142861</v>
       </c>
-      <c r="C3" s="26">
-        <f>G15*I4*N7%</f>
+      <c r="C3" s="25">
+        <f>G15*I4*P7%</f>
         <v>256</v>
       </c>
-      <c r="D3" s="26">
-        <f>G15*I5*N7%</f>
+      <c r="D3" s="25">
+        <f>G15*I5*P7%</f>
         <v>182.85714285714286</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <v>10000</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="31">
         <v>0.4</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="49">
+        <f>16960</f>
         <v>16960</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="K3" s="6">
+        <f>J3*L3</f>
+        <v>33920</v>
+      </c>
+      <c r="L3" s="6">
+        <v>2</v>
+      </c>
+      <c r="O3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="32">
+      <c r="P3" s="31">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26">
-        <f>G15*I3*N7%</f>
+      <c r="B4" s="25">
+        <f>G15*I3*P7%</f>
         <v>292.57142857142861</v>
       </c>
-      <c r="C4" s="26">
-        <f>G15*I4*N7%</f>
+      <c r="C4" s="25">
+        <f>G15*I4*P7%</f>
         <v>256</v>
       </c>
-      <c r="D4" s="26">
-        <f>G15*I5*N7%</f>
+      <c r="D4" s="25">
+        <f>G15*I5*P7%</f>
         <v>182.85714285714286</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>12000</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="31">
         <v>0.35</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="49">
+        <f>14790</f>
         <v>14790</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="K4" s="6">
+        <f>J4*L3</f>
+        <v>29580</v>
+      </c>
+      <c r="O4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="32">
+      <c r="P4" s="31">
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="26">
-        <f>G15*I3*N7%</f>
+      <c r="B5" s="25">
+        <f>G15*I3*P7%</f>
         <v>292.57142857142861</v>
       </c>
-      <c r="C5" s="26">
-        <f>G15*I4*N7%</f>
+      <c r="C5" s="25">
+        <f>G15*I4*P7%</f>
         <v>256</v>
       </c>
-      <c r="D5" s="26">
-        <f>G15*I5*N7%</f>
+      <c r="D5" s="25">
+        <f>G15*I5*P7%</f>
         <v>182.85714285714286</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>15000</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="31">
         <v>0.25</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="49">
+        <f>10440</f>
         <v>10440</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="K5" s="6">
+        <f>J5*L3</f>
+        <v>20880</v>
+      </c>
+      <c r="O5" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25">
+        <f>G15*I3*P4</f>
+        <v>819.20000000000016</v>
+      </c>
+      <c r="C6" s="25">
+        <f>G15*I4*P4</f>
+        <v>716.8</v>
+      </c>
+      <c r="D6" s="25">
+        <f>G15*I5*P4</f>
+        <v>512</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="31">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="25">
+        <f>G15*I3*P7%</f>
+        <v>292.57142857142861</v>
+      </c>
+      <c r="C7" s="25">
+        <f>G15*I4*P7%</f>
+        <v>256</v>
+      </c>
+      <c r="D7" s="25">
+        <f>G15*I5*P7%</f>
+        <v>182.85714285714286</v>
+      </c>
+      <c r="O7" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="26">
-        <f>G15*I3*N4</f>
-        <v>819.20000000000016</v>
-      </c>
-      <c r="C6" s="26">
-        <f>G15*I4*N4</f>
-        <v>716.8</v>
-      </c>
-      <c r="D6" s="26">
-        <f>G15*I5*N4</f>
-        <v>512</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="32">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="26">
-        <f>G15*I3*N7%</f>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C7" s="26">
-        <f>G15*I4*N7%</f>
-        <v>256</v>
-      </c>
-      <c r="D7" s="26">
-        <f>G15*I5*N7%</f>
-        <v>182.85714285714286</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="34">
+      <c r="P7" s="33">
         <f>30/7</f>
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="26">
-        <f>G15*I3*N5</f>
+      <c r="B8" s="25">
+        <f>G15*I3*P5</f>
         <v>682.66666666666686</v>
       </c>
-      <c r="C8" s="26">
-        <f>G15*I4*N5</f>
+      <c r="C8" s="25">
+        <f>G15*I4*P5</f>
         <v>597.33333333333337</v>
       </c>
-      <c r="D8" s="26">
-        <f>G15*I5*N5</f>
+      <c r="D8" s="25">
+        <f>G15*I5*P5</f>
         <v>426.66666666666674</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26">
-        <f>G15*I3*N5</f>
+      <c r="B9" s="25">
+        <f>G15*I3*P5</f>
         <v>682.66666666666686</v>
       </c>
-      <c r="C9" s="26">
-        <f>G15*I4*N5</f>
+      <c r="C9" s="25">
+        <f>G15*I4*P5</f>
         <v>597.33333333333337</v>
       </c>
-      <c r="D9" s="26">
-        <f>G15*I5*N5</f>
+      <c r="D9" s="25">
+        <f>G15*I5*P5</f>
         <v>426.66666666666674</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="26">
-        <f>G15*I3*N7%</f>
+      <c r="B10" s="25">
+        <f>G15*I3*P7%</f>
         <v>292.57142857142861</v>
       </c>
-      <c r="C10" s="26">
-        <f>G15*I4*N7%</f>
+      <c r="C10" s="25">
+        <f>G15*I4*P7%</f>
         <v>256</v>
       </c>
-      <c r="D10" s="26">
-        <f>G15*I5*N7%</f>
+      <c r="D10" s="25">
+        <f>G15*I5*P7%</f>
         <v>182.85714285714286</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="26">
-        <f>G15*I3*N7%</f>
+      <c r="B11" s="25">
+        <f>G15*I3*P7%</f>
         <v>292.57142857142861</v>
       </c>
-      <c r="C11" s="26">
-        <f>G15*I4*N7%</f>
+      <c r="C11" s="25">
+        <f>G15*I4*P7%</f>
         <v>256</v>
       </c>
-      <c r="D11" s="26">
-        <f>G15*I5*N7%</f>
+      <c r="D11" s="25">
+        <f>G15*I5*P7%</f>
         <v>182.85714285714286</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="26">
-        <f>G15*I3*N6</f>
+      <c r="B12" s="25">
+        <f>G15*I3*P6</f>
         <v>546.13333333333344</v>
       </c>
-      <c r="C12" s="26">
-        <f>G15*I4*N6</f>
+      <c r="C12" s="25">
+        <f>G15*I4*P6</f>
         <v>477.86666666666667</v>
       </c>
-      <c r="D12" s="26">
-        <f>G15*I5*N6</f>
+      <c r="D12" s="25">
+        <f>G15*I5*P6</f>
         <v>341.33333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="26">
-        <f>G15*I3*N7%</f>
+      <c r="B13" s="25">
+        <f>G15*I3*P7%</f>
         <v>292.57142857142861</v>
       </c>
-      <c r="C13" s="26">
-        <f>G15*I4*N7%</f>
+      <c r="C13" s="25">
+        <f>G15*I4*P7%</f>
         <v>256</v>
       </c>
-      <c r="D13" s="26">
-        <f>G15*I5*N7%</f>
+      <c r="D13" s="25">
+        <f>G15*I5*P7%</f>
         <v>182.85714285714286</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="26">
-        <f>G15*I3*N3</f>
+      <c r="B14" s="25">
+        <f>G15*I3*P3</f>
         <v>2048.0000000000005</v>
       </c>
-      <c r="C14" s="26">
-        <f>G15*I4*N3</f>
+      <c r="C14" s="25">
+        <f>G15*I4*P3</f>
         <v>1791.9999999999998</v>
       </c>
-      <c r="D14" s="26">
-        <f>G15*I5*N3</f>
+      <c r="D14" s="25">
+        <f>G15*I5*P3</f>
         <v>1280</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G15" s="6">
         <f>(800000)*(1+10*(2/3)/100)*0.02</f>
         <v>17066.666666666668</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="str">
         <f t="shared" ref="A18:D30" si="0">A2</f>
         <v>Mes</v>
@@ -6412,247 +7816,248 @@
         <v>Casa</v>
       </c>
       <c r="G18" s="6">
-        <f>G15*20%</f>
-        <v>3413.3333333333339</v>
+        <f>G15*G21</f>
+        <v>8533.3333333333339</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Enero</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <f>B3*1000000/$H$3</f>
         <v>29257.142857142859</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="22">
         <f>C3*1000000/$H$4</f>
         <v>21333.333333333332</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="22">
         <f>D3*1000000/$H$5</f>
         <v>12190.476190476191</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Febrero</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <f t="shared" ref="B20:B21" si="1">B4*1000000/$H$3</f>
         <v>29257.142857142859</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="22">
         <f t="shared" ref="C20:C30" si="2">C4*1000000/$H$4</f>
         <v>21333.333333333332</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <f t="shared" ref="D20:D30" si="3">D4*1000000/$H$5</f>
         <v>12190.476190476191</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Marzo</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <f t="shared" si="1"/>
         <v>29257.142857142859</v>
       </c>
-      <c r="C21" s="23">
-        <f t="shared" si="2"/>
+      <c r="C21" s="22">
+        <f>C5*1000000/$H$4</f>
         <v>21333.333333333332</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="22">
         <f t="shared" si="3"/>
         <v>12190.476190476191</v>
       </c>
-      <c r="G21" s="21">
-        <v>0.2</v>
+      <c r="G21" s="31">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Abril</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="22">
         <f>B6*1000000/$H$3</f>
         <v>81920.000000000015</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="22">
         <f t="shared" si="2"/>
         <v>59733.333333333336</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <f t="shared" si="3"/>
         <v>34133.333333333336</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Mayo</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="22">
         <f t="shared" ref="B23:B29" si="4">B7*1000000/$H$3</f>
         <v>29257.142857142859</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="22">
         <f t="shared" si="2"/>
         <v>21333.333333333332</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
         <f t="shared" si="3"/>
         <v>12190.476190476191</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Junio</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <f t="shared" si="4"/>
         <v>68266.666666666686</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="22">
         <f t="shared" si="2"/>
         <v>49777.777777777781</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <f t="shared" si="3"/>
         <v>28444.444444444449</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Julio</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="22">
         <f t="shared" si="4"/>
         <v>68266.666666666686</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="22">
         <f t="shared" si="2"/>
         <v>49777.777777777781</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <f t="shared" si="3"/>
         <v>28444.444444444449</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Agosto</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="22">
         <f>B10*1000000/$H$3</f>
         <v>29257.142857142859</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="22">
         <f t="shared" si="2"/>
         <v>21333.333333333332</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="22">
         <f t="shared" si="3"/>
         <v>12190.476190476191</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Septiembre</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="22">
         <f t="shared" si="4"/>
         <v>29257.142857142859</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="22">
         <f t="shared" si="2"/>
         <v>21333.333333333332</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="22">
         <f t="shared" si="3"/>
         <v>12190.476190476191</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Octubre</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <f t="shared" si="4"/>
         <v>54613.33333333335</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="22">
         <f t="shared" si="2"/>
         <v>39822.222222222226</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="22">
         <f t="shared" si="3"/>
         <v>22755.555555555558</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Noviembre</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <f t="shared" si="4"/>
         <v>29257.142857142859</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="22">
         <f t="shared" si="2"/>
         <v>21333.333333333332</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="22">
         <f t="shared" si="3"/>
         <v>12190.476190476191</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Diciembre</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="22">
         <f>B14*1000000/$H$3</f>
         <v>204800.00000000006</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="22">
         <f t="shared" si="2"/>
         <v>149333.33333333331</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="22">
         <f t="shared" si="3"/>
         <v>85333.333333333328</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="25.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="F33" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
+    <row r="33" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="F33" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="46"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="str">
         <f t="shared" ref="A34:D46" si="5">A18</f>
         <v>Mes</v>
@@ -6685,425 +8090,443 @@
         <f t="shared" ref="I34:I43" si="9">D34</f>
         <v>Casa</v>
       </c>
+      <c r="J34" s="47"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Enero</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <f>B19*$G$21</f>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C35" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C35" s="22">
         <f>C19*$G$21</f>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D35" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D35" s="22">
         <f>D19*$G$21</f>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F35" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Enero</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="22">
         <f t="shared" si="7"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="H35" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="H35" s="22">
         <f t="shared" si="8"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="I35" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="I35" s="22">
         <f t="shared" si="9"/>
-        <v>2438.0952380952381</v>
-      </c>
+        <v>6095.2380952380954</v>
+      </c>
+      <c r="J35" s="48"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Febrero</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="22">
         <f t="shared" ref="B36:D46" si="10">B20*$G$21</f>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C36" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C36" s="22">
         <f t="shared" si="10"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D36" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D36" s="22">
         <f t="shared" si="10"/>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F36" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Febrero</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="22">
         <f t="shared" si="7"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="H36" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="H36" s="22">
         <f t="shared" si="8"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="I36" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="I36" s="22">
         <f t="shared" si="9"/>
-        <v>2438.0952380952381</v>
-      </c>
+        <v>6095.2380952380954</v>
+      </c>
+      <c r="J36" s="48"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Marzo</v>
       </c>
-      <c r="B37" s="23">
+      <c r="B37" s="22">
         <f t="shared" si="10"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C37" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C37" s="22">
         <f t="shared" si="10"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D37" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D37" s="22">
         <f t="shared" si="10"/>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F37" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Marzo</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="22">
         <f>B37+B38-G38</f>
-        <v>7478.4285714285761</v>
-      </c>
-      <c r="H37" s="23">
-        <f t="shared" si="8"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="I37" s="23">
+        <v>21668.571428571435</v>
+      </c>
+      <c r="H37" s="22">
+        <f>C38-H38+C37</f>
+        <v>10666.666666666666</v>
+      </c>
+      <c r="I37" s="22">
         <f t="shared" si="9"/>
-        <v>2438.0952380952381</v>
-      </c>
+        <v>6095.2380952380954</v>
+      </c>
+      <c r="J37" s="48"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Abril</v>
       </c>
-      <c r="B38" s="23">
+      <c r="B38" s="22">
         <f t="shared" si="10"/>
-        <v>16384.000000000004</v>
-      </c>
-      <c r="C38" s="23">
+        <v>40960.000000000007</v>
+      </c>
+      <c r="C38" s="22">
         <f t="shared" si="10"/>
-        <v>11946.666666666668</v>
-      </c>
-      <c r="D38" s="23">
+        <v>29866.666666666668</v>
+      </c>
+      <c r="D38" s="22">
         <f t="shared" si="10"/>
-        <v>6826.6666666666679</v>
+        <v>17066.666666666668</v>
       </c>
       <c r="F38" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Abril</v>
       </c>
-      <c r="G38" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H38" s="23">
-        <f t="shared" si="8"/>
-        <v>11946.666666666668</v>
-      </c>
-      <c r="I38" s="23">
+      <c r="G38" s="22">
+        <f>K3</f>
+        <v>33920</v>
+      </c>
+      <c r="H38" s="22">
+        <f>C38</f>
+        <v>29866.666666666668</v>
+      </c>
+      <c r="I38" s="22">
         <f t="shared" si="9"/>
-        <v>6826.6666666666679</v>
-      </c>
+        <v>17066.666666666668</v>
+      </c>
+      <c r="J38" s="48"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Mayo</v>
       </c>
-      <c r="B39" s="23">
+      <c r="B39" s="22">
         <f t="shared" si="10"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C39" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C39" s="22">
         <f t="shared" si="10"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D39" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D39" s="22">
         <f t="shared" si="10"/>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F39" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Mayo</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="22">
         <f>B39+B40+B41-G40-G41</f>
-        <v>3644.095238095244</v>
-      </c>
-      <c r="H39" s="23">
+        <v>14628.57142857142</v>
+      </c>
+      <c r="H39" s="22">
         <f t="shared" si="8"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="I39" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="I39" s="22">
         <f t="shared" si="9"/>
-        <v>2438.0952380952381</v>
-      </c>
+        <v>6095.2380952380954</v>
+      </c>
+      <c r="J39" s="48"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Junio</v>
       </c>
-      <c r="B40" s="23">
+      <c r="B40" s="22">
         <f t="shared" si="10"/>
-        <v>13653.333333333338</v>
-      </c>
-      <c r="C40" s="23">
+        <v>34133.333333333343</v>
+      </c>
+      <c r="C40" s="22">
         <f t="shared" si="10"/>
-        <v>9955.5555555555566</v>
-      </c>
-      <c r="D40" s="23">
+        <v>24888.888888888891</v>
+      </c>
+      <c r="D40" s="22">
         <f t="shared" si="10"/>
-        <v>5688.8888888888905</v>
+        <v>14222.222222222224</v>
       </c>
       <c r="F40" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Junio</v>
       </c>
-      <c r="G40" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H40" s="23">
-        <f t="shared" si="8"/>
-        <v>9955.5555555555566</v>
-      </c>
-      <c r="I40" s="23">
+      <c r="G40" s="22">
+        <f>B40</f>
+        <v>34133.333333333343</v>
+      </c>
+      <c r="H40" s="22">
+        <f>C40</f>
+        <v>24888.888888888891</v>
+      </c>
+      <c r="I40" s="22">
         <f t="shared" si="9"/>
-        <v>5688.8888888888905</v>
-      </c>
+        <v>14222.222222222224</v>
+      </c>
+      <c r="J40" s="48"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Julio</v>
       </c>
-      <c r="B41" s="23">
+      <c r="B41" s="22">
         <f t="shared" si="10"/>
-        <v>13653.333333333338</v>
-      </c>
-      <c r="C41" s="23">
+        <v>34133.333333333343</v>
+      </c>
+      <c r="C41" s="22">
         <f t="shared" si="10"/>
-        <v>9955.5555555555566</v>
-      </c>
-      <c r="D41" s="23">
+        <v>24888.888888888891</v>
+      </c>
+      <c r="D41" s="22">
         <f t="shared" si="10"/>
-        <v>5688.8888888888905</v>
+        <v>14222.222222222224</v>
       </c>
       <c r="F41" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Julio</v>
       </c>
-      <c r="G41" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H41" s="23">
-        <f t="shared" si="8"/>
-        <v>9955.5555555555566</v>
-      </c>
-      <c r="I41" s="23">
+      <c r="G41" s="22">
+        <f>B41</f>
+        <v>34133.333333333343</v>
+      </c>
+      <c r="H41" s="22">
+        <f>C41</f>
+        <v>24888.888888888891</v>
+      </c>
+      <c r="I41" s="22">
         <f t="shared" si="9"/>
-        <v>5688.8888888888905</v>
-      </c>
+        <v>14222.222222222224</v>
+      </c>
+      <c r="J41" s="48"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Agosto</v>
       </c>
-      <c r="B42" s="23">
+      <c r="B42" s="22">
         <f t="shared" si="10"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C42" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C42" s="22">
         <f t="shared" si="10"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D42" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D42" s="22">
         <f t="shared" si="10"/>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F42" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Agosto</v>
       </c>
-      <c r="G42" s="23">
+      <c r="G42" s="22">
         <f>B42+SUM(B43:B46)-SUM(G43:G46)</f>
-        <v>10408.952380952396</v>
-      </c>
-      <c r="H42" s="23">
+        <v>37912.380952380976</v>
+      </c>
+      <c r="H42" s="22">
         <f t="shared" si="8"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="I42" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="I42" s="22">
         <f t="shared" si="9"/>
-        <v>2438.0952380952381</v>
-      </c>
+        <v>6095.2380952380954</v>
+      </c>
+      <c r="J42" s="48"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Septiembre</v>
       </c>
-      <c r="B43" s="23">
+      <c r="B43" s="22">
         <f t="shared" si="10"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C43" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C43" s="22">
         <f t="shared" si="10"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D43" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D43" s="22">
         <f t="shared" si="10"/>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F43" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Septiembre</v>
       </c>
-      <c r="G43" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H43" s="23">
+      <c r="G43" s="22">
+        <f>K3</f>
+        <v>33920</v>
+      </c>
+      <c r="H43" s="22">
         <f>C43+SUM(C44:C46)-SUM(H44:H46)</f>
-        <v>7745.4444444444453</v>
-      </c>
-      <c r="I43" s="23">
+        <v>27171.111111111109</v>
+      </c>
+      <c r="I43" s="22">
         <f t="shared" si="9"/>
-        <v>2438.0952380952381</v>
-      </c>
+        <v>6095.2380952380954</v>
+      </c>
+      <c r="J43" s="48"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Octubre</v>
       </c>
-      <c r="B44" s="23">
+      <c r="B44" s="22">
         <f t="shared" si="10"/>
-        <v>10922.666666666672</v>
-      </c>
-      <c r="C44" s="23">
+        <v>27306.666666666675</v>
+      </c>
+      <c r="C44" s="22">
         <f t="shared" si="10"/>
-        <v>7964.4444444444453</v>
-      </c>
-      <c r="D44" s="23">
+        <v>19911.111111111113</v>
+      </c>
+      <c r="D44" s="22">
         <f t="shared" si="10"/>
-        <v>4551.1111111111122</v>
+        <v>11377.777777777779</v>
       </c>
       <c r="F44" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Octubre</v>
       </c>
-      <c r="G44" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H44" s="23">
-        <v>12873</v>
-      </c>
-      <c r="I44" s="23">
+      <c r="G44" s="22">
+        <f>K3</f>
+        <v>33920</v>
+      </c>
+      <c r="H44" s="22">
+        <f>K4</f>
+        <v>29580</v>
+      </c>
+      <c r="I44" s="22">
         <f>D44+SUM(D45:D46)-SUM(I45:I46)</f>
-        <v>5883.8730158730177</v>
-      </c>
+        <v>18379.682539682544</v>
+      </c>
+      <c r="J44" s="48"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Noviembre</v>
       </c>
-      <c r="B45" s="23">
+      <c r="B45" s="22">
         <f t="shared" si="10"/>
-        <v>5851.4285714285725</v>
-      </c>
-      <c r="C45" s="23">
+        <v>14628.571428571429</v>
+      </c>
+      <c r="C45" s="22">
         <f t="shared" si="10"/>
-        <v>4266.666666666667</v>
-      </c>
-      <c r="D45" s="23">
+        <v>10666.666666666666</v>
+      </c>
+      <c r="D45" s="22">
         <f t="shared" si="10"/>
-        <v>2438.0952380952381</v>
+        <v>6095.2380952380954</v>
       </c>
       <c r="F45" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Noviembre</v>
       </c>
-      <c r="G45" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H45" s="23">
-        <v>12873</v>
-      </c>
-      <c r="I45" s="23">
-        <v>9086</v>
-      </c>
+      <c r="G45" s="22">
+        <f>K3</f>
+        <v>33920</v>
+      </c>
+      <c r="H45" s="22">
+        <f>K4</f>
+        <v>29580</v>
+      </c>
+      <c r="I45" s="22">
+        <f>K5</f>
+        <v>20880</v>
+      </c>
+      <c r="J45" s="48"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Diciembre</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="22">
+        <f>B30*$G$21</f>
+        <v>102400.00000000003</v>
+      </c>
+      <c r="C46" s="22">
         <f t="shared" si="10"/>
-        <v>40960.000000000015</v>
-      </c>
-      <c r="C46" s="23">
+        <v>74666.666666666657</v>
+      </c>
+      <c r="D46" s="22">
         <f t="shared" si="10"/>
-        <v>29866.666666666664</v>
-      </c>
-      <c r="D46" s="23">
-        <f t="shared" si="10"/>
-        <v>17066.666666666668</v>
+        <v>42666.666666666664</v>
       </c>
       <c r="F46" s="6" t="str">
         <f t="shared" si="6"/>
         <v>Diciembre</v>
       </c>
-      <c r="G46" s="23">
-        <f>14757</f>
-        <v>14757</v>
-      </c>
-      <c r="H46" s="23">
-        <v>12873</v>
-      </c>
-      <c r="I46" s="23">
-        <v>9086</v>
-      </c>
+      <c r="G46" s="22">
+        <f>K3</f>
+        <v>33920</v>
+      </c>
+      <c r="H46" s="22">
+        <f>K4</f>
+        <v>29580</v>
+      </c>
+      <c r="I46" s="22">
+        <f>K5</f>
+        <v>20880</v>
+      </c>
+      <c r="J46" s="48"/>
     </row>
-    <row r="49" spans="1:7" ht="25.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="41" t="str">
+    <row r="49" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="40" t="str">
         <f t="shared" ref="A49:D62" si="11">A1</f>
         <v>Estimación ventas mensuales por tipo de juguete (Millones COP)</v>
       </c>
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="43"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="42"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Mes</v>
       </c>
-      <c r="B50" s="23" t="str">
+      <c r="B50" s="22" t="str">
         <f t="shared" si="11"/>
         <v>Moto</v>
       </c>
@@ -7115,223 +8538,223 @@
         <f t="shared" si="11"/>
         <v>Casa</v>
       </c>
-      <c r="G50" s="22"/>
+      <c r="G50" s="21"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Enero</v>
       </c>
-      <c r="B51" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C51" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D51" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
+      <c r="B51" s="22">
+        <f>B3*$G$21</f>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C51" s="22">
+        <f>C3*$G$21</f>
+        <v>128</v>
+      </c>
+      <c r="D51" s="22">
+        <f>D3*$G$21</f>
+        <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Febrero</v>
       </c>
-      <c r="B52" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C52" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D52" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
+      <c r="B52" s="22">
+        <f t="shared" ref="B52:B62" si="12">B4*$G$21</f>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C52" s="22">
+        <f t="shared" ref="C52:C62" si="13">C4*$G$21</f>
+        <v>128</v>
+      </c>
+      <c r="D52" s="22">
+        <f t="shared" ref="D52:D62" si="14">D4*$G$21</f>
+        <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Marzo</v>
       </c>
-      <c r="B53" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C53" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D53" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
-      </c>
-      <c r="G53" s="22"/>
+      <c r="B53" s="22">
+        <f t="shared" si="12"/>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C53" s="22">
+        <f t="shared" si="13"/>
+        <v>128</v>
+      </c>
+      <c r="D53" s="22">
+        <f t="shared" si="14"/>
+        <v>91.428571428571431</v>
+      </c>
+      <c r="G53" s="21"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Abril</v>
       </c>
-      <c r="B54" s="23">
-        <f t="shared" si="11"/>
-        <v>819.20000000000016</v>
-      </c>
-      <c r="C54" s="23">
-        <f t="shared" si="11"/>
-        <v>716.8</v>
-      </c>
-      <c r="D54" s="23">
-        <f t="shared" si="11"/>
-        <v>512</v>
+      <c r="B54" s="22">
+        <f t="shared" si="12"/>
+        <v>409.60000000000008</v>
+      </c>
+      <c r="C54" s="22">
+        <f t="shared" si="13"/>
+        <v>358.4</v>
+      </c>
+      <c r="D54" s="22">
+        <f t="shared" si="14"/>
+        <v>256</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Mayo</v>
       </c>
-      <c r="B55" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C55" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D55" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
+      <c r="B55" s="22">
+        <f t="shared" si="12"/>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C55" s="22">
+        <f t="shared" si="13"/>
+        <v>128</v>
+      </c>
+      <c r="D55" s="22">
+        <f t="shared" si="14"/>
+        <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Junio</v>
       </c>
-      <c r="B56" s="23">
-        <f t="shared" si="11"/>
-        <v>682.66666666666686</v>
-      </c>
-      <c r="C56" s="23">
-        <f t="shared" si="11"/>
-        <v>597.33333333333337</v>
-      </c>
-      <c r="D56" s="23">
-        <f t="shared" si="11"/>
-        <v>426.66666666666674</v>
+      <c r="B56" s="22">
+        <f t="shared" si="12"/>
+        <v>341.33333333333343</v>
+      </c>
+      <c r="C56" s="22">
+        <f t="shared" si="13"/>
+        <v>298.66666666666669</v>
+      </c>
+      <c r="D56" s="22">
+        <f t="shared" si="14"/>
+        <v>213.33333333333337</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Julio</v>
       </c>
-      <c r="B57" s="23">
-        <f t="shared" si="11"/>
-        <v>682.66666666666686</v>
-      </c>
-      <c r="C57" s="23">
-        <f t="shared" si="11"/>
-        <v>597.33333333333337</v>
-      </c>
-      <c r="D57" s="23">
-        <f t="shared" si="11"/>
-        <v>426.66666666666674</v>
+      <c r="B57" s="22">
+        <f t="shared" si="12"/>
+        <v>341.33333333333343</v>
+      </c>
+      <c r="C57" s="22">
+        <f t="shared" si="13"/>
+        <v>298.66666666666669</v>
+      </c>
+      <c r="D57" s="22">
+        <f t="shared" si="14"/>
+        <v>213.33333333333337</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Agosto</v>
       </c>
-      <c r="B58" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C58" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D58" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
+      <c r="B58" s="22">
+        <f t="shared" si="12"/>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C58" s="22">
+        <f t="shared" si="13"/>
+        <v>128</v>
+      </c>
+      <c r="D58" s="22">
+        <f t="shared" si="14"/>
+        <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Septiembre</v>
       </c>
-      <c r="B59" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C59" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D59" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
+      <c r="B59" s="22">
+        <f t="shared" si="12"/>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C59" s="22">
+        <f t="shared" si="13"/>
+        <v>128</v>
+      </c>
+      <c r="D59" s="22">
+        <f t="shared" si="14"/>
+        <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Octubre</v>
       </c>
-      <c r="B60" s="23">
-        <f t="shared" si="11"/>
-        <v>546.13333333333344</v>
-      </c>
-      <c r="C60" s="23">
-        <f t="shared" si="11"/>
-        <v>477.86666666666667</v>
-      </c>
-      <c r="D60" s="23">
-        <f t="shared" si="11"/>
-        <v>341.33333333333337</v>
+      <c r="B60" s="22">
+        <f t="shared" si="12"/>
+        <v>273.06666666666672</v>
+      </c>
+      <c r="C60" s="22">
+        <f t="shared" si="13"/>
+        <v>238.93333333333334</v>
+      </c>
+      <c r="D60" s="22">
+        <f t="shared" si="14"/>
+        <v>170.66666666666669</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Noviembre</v>
       </c>
-      <c r="B61" s="23">
-        <f t="shared" si="11"/>
-        <v>292.57142857142861</v>
-      </c>
-      <c r="C61" s="23">
-        <f t="shared" si="11"/>
-        <v>256</v>
-      </c>
-      <c r="D61" s="23">
-        <f t="shared" si="11"/>
-        <v>182.85714285714286</v>
+      <c r="B61" s="22">
+        <f>B13*$G$21</f>
+        <v>146.28571428571431</v>
+      </c>
+      <c r="C61" s="22">
+        <f t="shared" si="13"/>
+        <v>128</v>
+      </c>
+      <c r="D61" s="22">
+        <f t="shared" si="14"/>
+        <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Diciembre</v>
       </c>
-      <c r="B62" s="23">
-        <f t="shared" si="11"/>
-        <v>2048.0000000000005</v>
-      </c>
-      <c r="C62" s="23">
-        <f t="shared" si="11"/>
-        <v>1791.9999999999998</v>
-      </c>
-      <c r="D62" s="23">
-        <f t="shared" si="11"/>
-        <v>1280</v>
+      <c r="B62" s="22">
+        <f t="shared" si="12"/>
+        <v>1024.0000000000002</v>
+      </c>
+      <c r="C62" s="22">
+        <f t="shared" si="13"/>
+        <v>895.99999999999989</v>
+      </c>
+      <c r="D62" s="22">
+        <f t="shared" si="14"/>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -7340,7 +8763,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A33:D33"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="F33:I33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7357,51 +8780,51 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" style="1" customWidth="1"/>
-    <col min="8" max="12" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.453125" style="1"/>
+    <col min="2" max="2" width="15.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8" max="12" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="10">
-        <f>3413.333333*1000000</f>
-        <v>3413333333</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37">
+        <f>'Proyección ventas'!G18*1000000</f>
+        <v>8533333333.333334</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="E2" s="37">
+      <c r="E2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="G2" s="2">
         <v>0.12</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="I2" s="2">
@@ -7410,23 +8833,23 @@
       <c r="J2" s="2">
         <v>0.1</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="L2" s="37">
+      <c r="L2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="M2" s="2">
         <v>0.08</v>
       </c>
-      <c r="N2" s="37">
+      <c r="N2" s="36">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="O2" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -7473,252 +8896,254 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="35">
-        <f>B2/12000</f>
-        <v>284444.44441666669</v>
+      <c r="B4" s="34">
+        <f>B2*C4/'Proyección ventas'!H4</f>
+        <v>248888.88888888888</v>
       </c>
       <c r="C4" s="7">
+        <f>'Proyección ventas'!I4</f>
         <v>0.35</v>
       </c>
       <c r="D4" s="11">
         <f>+C4*$B$2*$D$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="E4" s="11">
         <f>C4*$B$2*$E$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="F4" s="12">
         <f>C4*$B$2*$F$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="G4" s="12">
         <f>C4*$B$2*$G$2</f>
-        <v>143359999.986</v>
+        <v>358399999.99999994</v>
       </c>
       <c r="H4" s="12">
         <f>C4*$B$2*$H$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="I4" s="12">
         <f>C4*$B$2*$I$2</f>
-        <v>119466666.655</v>
+        <v>298666666.66666669</v>
       </c>
       <c r="J4" s="12">
         <f>C4*$B$2*$J$2</f>
-        <v>119466666.655</v>
+        <v>298666666.66666669</v>
       </c>
       <c r="K4" s="12">
         <f>C4*$B$2*$K$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="L4" s="12">
         <f>C4*$B$2*$L$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="M4" s="12">
         <f>C4*$B$2*$M$2</f>
-        <v>95573333.324000001</v>
+        <v>238933333.33333331</v>
       </c>
       <c r="N4" s="12">
         <f>C4*$B$2*$N$2</f>
-        <v>51370666.661649995</v>
+        <v>128426666.66666666</v>
       </c>
       <c r="O4" s="12">
         <f>C4*$B$2*$O$2</f>
-        <v>358399999.96499997</v>
+        <v>895999999.99999988</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="35">
-        <f>B2/15000</f>
-        <v>227555.55553333333</v>
+      <c r="B5" s="34">
+        <f>B2/'Proyección ventas'!H5</f>
+        <v>568888.88888888888</v>
       </c>
       <c r="C5" s="7">
+        <f>'Proyección ventas'!I5</f>
         <v>0.25</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" ref="D5:D6" si="0">+C5*$B$2*$D$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" ref="E5:E6" si="1">C5*$B$2*$E$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" ref="F5:F6" si="2">C5*$B$2*$F$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="G5" s="12">
         <f>C5*$B$2*$G$2</f>
-        <v>102399999.98999999</v>
+        <v>256000000</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" ref="H5:H6" si="3">C5*$B$2*$H$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" ref="I5:I6" si="4">C5*$B$2*$I$2</f>
-        <v>85333333.325000003</v>
+        <v>213333333.33333337</v>
       </c>
       <c r="J5" s="12">
         <f>C5*$B$2*$J$2</f>
-        <v>85333333.325000003</v>
+        <v>213333333.33333337</v>
       </c>
       <c r="K5" s="12">
         <f t="shared" ref="K5:K6" si="5">C5*$B$2*$K$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="L5" s="12">
         <f t="shared" ref="L5:L6" si="6">C5*$B$2*$L$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="M5" s="12">
         <f t="shared" ref="M5:M6" si="7">C5*$B$2*$M$2</f>
-        <v>68266666.659999996</v>
+        <v>170666666.66666669</v>
       </c>
       <c r="N5" s="12">
         <f t="shared" ref="N5:N6" si="8">C5*$B$2*$N$2</f>
-        <v>36693333.329749994</v>
+        <v>91733333.333333328</v>
       </c>
       <c r="O5" s="12">
         <f>C5*$B$2*$O$2</f>
-        <v>255999999.97499999</v>
+        <v>640000000</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="35">
-        <f>B2/10000</f>
-        <v>341333.3333</v>
+      <c r="B6" s="34">
+        <f>B2*40%/'Proyección ventas'!H3</f>
+        <v>341333.33333333337</v>
       </c>
       <c r="C6" s="7">
-        <f>+B6/$B$7</f>
-        <v>0.39999999999999997</v>
+        <f>'Proyección ventas'!I3</f>
+        <v>0.4</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="G6" s="12">
         <f>C6*$B$2*$G$2</f>
-        <v>163839999.98399997</v>
+        <v>409600000.00000006</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="3"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="4"/>
-        <v>136533333.31999999</v>
+        <v>341333333.33333343</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" ref="J6" si="9">C6*$B$2*$J$2</f>
-        <v>136533333.31999999</v>
+        <v>341333333.33333343</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" si="5"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="L6" s="12">
         <f t="shared" si="6"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="M6" s="12">
         <f t="shared" si="7"/>
-        <v>109226666.65599999</v>
+        <v>273066666.66666675</v>
       </c>
       <c r="N6" s="12">
         <f t="shared" si="8"/>
-        <v>58709333.327599987</v>
+        <v>146773333.33333334</v>
       </c>
       <c r="O6" s="12">
         <f>C6*$B$2*$O$2</f>
-        <v>409599999.95999992</v>
+        <v>1024000000.0000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="14">
         <f>SUM(B4:B6)</f>
-        <v>853333.33325000003</v>
+        <v>1159111.111111111</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13">
         <f t="shared" ref="D7:O7" si="10">SUM(D4:D6)</f>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="10"/>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="F7" s="13">
         <f t="shared" si="10"/>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="G7" s="13">
         <f t="shared" si="10"/>
-        <v>409599999.95999998</v>
+        <v>1024000000</v>
       </c>
       <c r="H7" s="13">
         <f t="shared" si="10"/>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="I7" s="13">
         <f t="shared" si="10"/>
-        <v>341333333.30000001</v>
+        <v>853333333.33333349</v>
       </c>
       <c r="J7" s="13">
         <f t="shared" si="10"/>
-        <v>341333333.30000001</v>
+        <v>853333333.33333349</v>
       </c>
       <c r="K7" s="13">
         <f t="shared" si="10"/>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="L7" s="13">
         <f t="shared" si="10"/>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="M7" s="13">
         <f t="shared" si="10"/>
-        <v>273066666.63999999</v>
+        <v>682666666.66666675</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="10"/>
-        <v>146773333.31899998</v>
+        <v>366933333.33333337</v>
       </c>
       <c r="O7" s="13">
         <f t="shared" si="10"/>
-        <v>1023999999.8999999</v>
+        <v>2560000000</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>31</v>
       </c>
@@ -7727,54 +9152,54 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:O9" si="11">+$C$9*D7</f>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="11"/>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="11"/>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="11"/>
-        <v>61439999.993999995</v>
+        <v>153600000</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="11"/>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="11"/>
-        <v>51199999.994999997</v>
+        <v>128000000.00000001</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="11"/>
-        <v>51199999.994999997</v>
+        <v>128000000.00000001</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="11"/>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="11"/>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="11"/>
-        <v>40959999.995999999</v>
+        <v>102400000.00000001</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="11"/>
-        <v>22015999.997849997</v>
+        <v>55040000.000000007</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="11"/>
-        <v>153599999.98499998</v>
+        <v>384000000</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -7783,220 +9208,233 @@
       </c>
       <c r="D10" s="1">
         <f>+$C$10*D7</f>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10:O10" si="12">+$C$10*E7</f>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="12"/>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="12"/>
-        <v>12287999.998799998</v>
+        <v>30720000</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="12"/>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="12"/>
-        <v>10239999.999</v>
+        <v>25600000.000000004</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="12"/>
-        <v>10239999.999</v>
+        <v>25600000.000000004</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="12"/>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="12"/>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="12"/>
-        <v>8191999.9991999995</v>
+        <v>20480000</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="12"/>
-        <v>4403199.9995699991</v>
+        <v>11008000</v>
       </c>
       <c r="O10" s="1">
         <f t="shared" si="12"/>
-        <v>30719999.996999994</v>
+        <v>76800000</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="1">
-        <f>10*1400000</f>
-        <v>14000000</v>
+        <f>10*1400000*'Proyección ventas'!L3</f>
+        <v>28000000</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" ref="D12:O12" si="13">+$C$12</f>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="13"/>
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="1">
-        <v>13000000</v>
+        <f>4000000+1000000</f>
+        <v>5000000</v>
       </c>
       <c r="D13" s="1">
-        <v>14000000</v>
+        <f>$C$13</f>
+        <v>5000000</v>
       </c>
       <c r="E13" s="1">
-        <v>14000000</v>
+        <f t="shared" ref="E13:O13" si="14">$C$13</f>
+        <v>5000000</v>
       </c>
       <c r="F13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="G13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="H13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="I13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="J13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="K13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="L13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="M13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="N13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
       <c r="O13" s="1">
-        <v>14000000</v>
+        <f t="shared" si="14"/>
+        <v>5000000</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:O14" si="14">+D7-D9-D12-D13-D10</f>
-        <v>92354133.321579978</v>
+        <f t="shared" ref="D14:O14" si="15">+D7-D9-D12-D13-D10</f>
+        <v>267885333.33333337</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="14"/>
-        <v>92354133.321579978</v>
+        <f t="shared" si="15"/>
+        <v>267885333.33333337</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="14"/>
-        <v>92354133.321579978</v>
+        <f t="shared" si="15"/>
+        <v>267885333.33333337</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="14"/>
-        <v>307871999.96719998</v>
+        <f t="shared" si="15"/>
+        <v>806680000</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="14"/>
-        <v>92354133.321579978</v>
+        <f t="shared" si="15"/>
+        <v>267885333.33333337</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="14"/>
-        <v>251893333.30599999</v>
+        <f t="shared" si="15"/>
+        <v>666733333.33333349</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="14"/>
-        <v>251893333.30599999</v>
+        <f t="shared" si="15"/>
+        <v>666733333.33333349</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="14"/>
-        <v>92354133.321579978</v>
+        <f t="shared" si="15"/>
+        <v>267885333.33333337</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="14"/>
-        <v>92354133.321579978</v>
+        <f t="shared" si="15"/>
+        <v>267885333.33333337</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="14"/>
-        <v>195914666.64480001</v>
+        <f t="shared" si="15"/>
+        <v>526786666.66666675</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="14"/>
-        <v>92354133.321579978</v>
+        <f t="shared" si="15"/>
+        <v>267885333.33333337</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="14"/>
-        <v>811679999.91799986</v>
+        <f t="shared" si="15"/>
+        <v>2066200000</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -8004,156 +9442,157 @@
         <v>0.35</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:O16" si="15">+IF(D14&lt;0,0,D14*$C$16)</f>
-        <v>32323946.66255299</v>
+        <f t="shared" ref="D16:O16" si="16">+IF(D14&lt;0,0,D14*$C$16)</f>
+        <v>93759866.666666672</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="15"/>
-        <v>32323946.66255299</v>
+        <f t="shared" si="16"/>
+        <v>93759866.666666672</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="15"/>
-        <v>32323946.66255299</v>
+        <f t="shared" si="16"/>
+        <v>93759866.666666672</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="15"/>
-        <v>107755199.98851998</v>
+        <f t="shared" si="16"/>
+        <v>282338000</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="15"/>
-        <v>32323946.66255299</v>
+        <f t="shared" si="16"/>
+        <v>93759866.666666672</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="15"/>
-        <v>88162666.657099992</v>
+        <f t="shared" si="16"/>
+        <v>233356666.66666672</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="15"/>
-        <v>88162666.657099992</v>
+        <f t="shared" si="16"/>
+        <v>233356666.66666672</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="15"/>
-        <v>32323946.66255299</v>
+        <f t="shared" si="16"/>
+        <v>93759866.666666672</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="15"/>
-        <v>32323946.66255299</v>
+        <f t="shared" si="16"/>
+        <v>93759866.666666672</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="15"/>
-        <v>68570133.325680003</v>
+        <f t="shared" si="16"/>
+        <v>184375333.33333334</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="15"/>
-        <v>32323946.66255299</v>
+        <f t="shared" si="16"/>
+        <v>93759866.666666672</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="15"/>
-        <v>284087999.97129995</v>
+        <f t="shared" si="16"/>
+        <v>723170000</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13">
         <f>+B18+B19</f>
-        <v>-1030000000</v>
+        <v>-1016000000</v>
       </c>
       <c r="D17" s="13">
-        <f t="shared" ref="D17:O17" si="16">+D14-D16</f>
-        <v>60030186.659026988</v>
+        <f t="shared" ref="D17:O17" si="17">+D14-D16</f>
+        <v>174125466.66666669</v>
       </c>
       <c r="E17" s="13">
-        <f t="shared" si="16"/>
-        <v>60030186.659026988</v>
+        <f t="shared" si="17"/>
+        <v>174125466.66666669</v>
       </c>
       <c r="F17" s="13">
-        <f t="shared" si="16"/>
-        <v>60030186.659026988</v>
+        <f t="shared" si="17"/>
+        <v>174125466.66666669</v>
       </c>
       <c r="G17" s="13">
-        <f t="shared" si="16"/>
-        <v>200116799.97868001</v>
+        <f t="shared" si="17"/>
+        <v>524342000</v>
       </c>
       <c r="H17" s="13">
-        <f t="shared" si="16"/>
-        <v>60030186.659026988</v>
+        <f t="shared" si="17"/>
+        <v>174125466.66666669</v>
       </c>
       <c r="I17" s="13">
-        <f t="shared" si="16"/>
-        <v>163730666.6489</v>
+        <f t="shared" si="17"/>
+        <v>433376666.66666675</v>
       </c>
       <c r="J17" s="13">
-        <f t="shared" si="16"/>
-        <v>163730666.6489</v>
+        <f t="shared" si="17"/>
+        <v>433376666.66666675</v>
       </c>
       <c r="K17" s="13">
-        <f t="shared" si="16"/>
-        <v>60030186.659026988</v>
+        <f t="shared" si="17"/>
+        <v>174125466.66666669</v>
       </c>
       <c r="L17" s="13">
-        <f t="shared" si="16"/>
-        <v>60030186.659026988</v>
+        <f t="shared" si="17"/>
+        <v>174125466.66666669</v>
       </c>
       <c r="M17" s="13">
-        <f t="shared" si="16"/>
-        <v>127344533.31912</v>
+        <f t="shared" si="17"/>
+        <v>342411333.33333337</v>
       </c>
       <c r="N17" s="13">
-        <f t="shared" si="16"/>
-        <v>60030186.659026988</v>
+        <f t="shared" si="17"/>
+        <v>174125466.66666669</v>
       </c>
       <c r="O17" s="13">
-        <f t="shared" si="16"/>
-        <v>527591999.94669992</v>
+        <f t="shared" si="17"/>
+        <v>1343030000</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1">
         <v>-1000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="38" t="s">
-        <v>55</v>
+    <row r="19" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="B19" s="1">
-        <v>-30000000</v>
+        <f>-8*5*100000*4</f>
+        <v>-16000000</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="16">
         <f>+NPV($B$23,D17:O17)</f>
-        <v>1100074225.984221</v>
+        <v>2963346767.125103</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="16">
         <f>+B20+B18+B19</f>
-        <v>70074225.984220982</v>
+        <v>1947346767.125103</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="17">
         <f>+IRR(C17:O17)</f>
-        <v>5.9470754636769207E-2</v>
+        <v>0.24923232879297297</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -8162,21 +9601,21 @@
       </c>
       <c r="C23" s="18"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="M25" s="39"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M25" s="38"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="M26" s="40"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M26" s="39"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="M27" s="40"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M27" s="39"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="M28" s="40"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M28" s="39"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>